<commit_message>
test vaxRestart with cases and seroprev
</commit_message>
<xml_diff>
--- a/Inputs/CAcounties_sigmaobs.xlsx
+++ b/Inputs/CAcounties_sigmaobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA12CB7-CDFA-0A41-B7EB-9CA9DD986AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99BED34-0CEA-AE4F-AE83-A33BC297F6B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="3340" windowWidth="29440" windowHeight="17100" activeTab="5" xr2:uid="{50240998-A895-7F42-B834-945925070EED}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="PUI Details" sheetId="7" r:id="rId5"/>
     <sheet name="Internal" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1000" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
   <si>
     <t>Number of Days from Infection to Becoming Infectious (Latent Period)</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Cumulative Hospitalizations</t>
   </si>
   <si>
-    <t>total admits to date</t>
-  </si>
-  <si>
     <t>PUI</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>deaths.conf</t>
   </si>
   <si>
-    <t>cum.admits.conf</t>
-  </si>
-  <si>
     <t>hosp.pui</t>
   </si>
   <si>
@@ -230,9 +224,6 @@
     <t>deaths.pui</t>
   </si>
   <si>
-    <t>cum.admits.pui</t>
-  </si>
-  <si>
     <t>mu_t_inter</t>
   </si>
   <si>
@@ -266,9 +257,6 @@
     <t>deaths</t>
   </si>
   <si>
-    <t>cum.admits</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fraction of PUI that are COVID+ </t>
   </si>
   <si>
@@ -282,15 +270,36 @@
   </si>
   <si>
     <t>automatic.interventions</t>
+  </si>
+  <si>
+    <t>frac_tested</t>
+  </si>
+  <si>
+    <t>sigma_obs_seroprev</t>
+  </si>
+  <si>
+    <t>admits</t>
+  </si>
+  <si>
+    <t>cases</t>
+  </si>
+  <si>
+    <t>seroprev</t>
+  </si>
+  <si>
+    <t>admits.conf</t>
+  </si>
+  <si>
+    <t>admits.pui</t>
+  </si>
+  <si>
+    <t>New Admits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000%"/>
-  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -537,8 +546,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -888,7 +899,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,15 +918,15 @@
         <v>20</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>11</v>
@@ -929,7 +940,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>0</v>
@@ -943,7 +954,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>1</v>
@@ -952,12 +963,12 @@
         <v>5</v>
       </c>
       <c r="D4" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>2</v>
@@ -966,32 +977,32 @@
         <v>6</v>
       </c>
       <c r="D5" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -999,7 +1010,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>3</v>
@@ -1008,18 +1019,18 @@
         <v>0.04</v>
       </c>
       <c r="D8" s="4">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="4">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="D9" s="4">
         <v>0.03</v>
@@ -1027,10 +1038,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="4">
         <v>0.5</v>
@@ -1040,7 +1051,15 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="35"/>
+      <c r="A11" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="36">
+        <v>0.05</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1074,56 +1093,56 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:6" s="28" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>69</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1147,43 +1166,43 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="35"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="36"/>
+      <c r="A6" s="35"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
+      <c r="A7" s="35"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="35"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="36"/>
+      <c r="A9" s="35"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="36"/>
+      <c r="A10" s="35"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="36"/>
+      <c r="A11" s="35"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="36"/>
+      <c r="A12" s="35"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="36"/>
+      <c r="A13" s="35"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="36"/>
+      <c r="A14" s="35"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="36"/>
+      <c r="A15" s="35"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="36"/>
+      <c r="A16" s="35"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36"/>
+      <c r="A17" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1280,7 +1299,7 @@
   <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1309,7 +1328,7 @@
       </c>
       <c r="G1" s="42"/>
       <c r="H1" s="38" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="I1" s="38"/>
     </row>
@@ -1327,7 +1346,7 @@
       </c>
       <c r="G2" s="43"/>
       <c r="H2" s="39" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="I2" s="39"/>
     </row>
@@ -1339,25 +1358,25 @@
         <v>31</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>31</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>31</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>31</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.2">
@@ -1365,28 +1384,28 @@
         <v>28</v>
       </c>
       <c r="B4" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="E4" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>65</v>
-      </c>
       <c r="H4" s="32" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4678,7 +4697,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4691,12 +4710,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4704,7 +4723,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" s="44" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D4" s="45"/>
     </row>
@@ -4716,15 +4735,15 @@
         <v>20</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>25</v>
@@ -4738,7 +4757,7 @@
     </row>
     <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>26</v>
@@ -4752,7 +4771,7 @@
     </row>
     <row r="8" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
@@ -4766,7 +4785,7 @@
     </row>
     <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
@@ -4778,8 +4797,28 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.05</v>
+      </c>
+    </row>
     <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -4787,7 +4826,7 @@
     <mergeCell ref="C4:D4"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:D9" xr:uid="{16C39E30-A382-9841-B9C1-7BE92A80BACE}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:D11" xr:uid="{16C39E30-A382-9841-B9C1-7BE92A80BACE}">
       <formula1>0</formula1>
       <formula2>20</formula2>
     </dataValidation>
@@ -4798,10 +4837,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DD5F9C-4676-5749-AB11-9739EC646DB2}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4819,7 +4858,7 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -4842,7 +4881,7 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>19</v>
@@ -4859,7 +4898,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4884,7 +4923,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -4898,15 +4937,15 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C8">
         <v>1000</v>
@@ -4914,19 +4953,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1500</v>
+      </c>
       <c r="C9" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3">
         <v>250</v>
@@ -4937,7 +4978,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3">
         <v>15</v>
@@ -4948,7 +4989,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3">
         <v>0.9</v>
@@ -4959,7 +5000,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B13" s="34">
         <v>0.3</v>
@@ -4970,10 +5011,18 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B14" s="34">
         <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="34">
+        <v>1E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>